<commit_message>
simplificamos el modelo del caso 1, habiamos creado una tabla demás
</commit_message>
<xml_diff>
--- a/modelo_lógico_datos_desafio_caso_1.xlsx
+++ b/modelo_lógico_datos_desafio_caso_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ariel/Desktop/desafiolatam/bases_de_datos_introducción/normalizacion_de_datos/modelos_desafio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D4F01A-EC27-1845-9D7C-799248EAAA3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38B1238-0E48-B640-851C-022D8C2CC591}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26140" yWindow="-3660" windowWidth="25040" windowHeight="14500" xr2:uid="{8EF448B2-BB9E-9141-B6BF-BD7A6BA49018}"/>
+    <workbookView xWindow="460" yWindow="860" windowWidth="25040" windowHeight="14500" xr2:uid="{8EF448B2-BB9E-9141-B6BF-BD7A6BA49018}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Departamentos</t>
   </si>
@@ -60,19 +60,10 @@
     <t>id_departamento [FK] NOT NULL</t>
   </si>
   <si>
-    <t>archivo_drive VARCHAR(20)</t>
-  </si>
-  <si>
     <t>rut_trabajador [FK] NOT NULL</t>
   </si>
   <si>
-    <t>archivos drive</t>
-  </si>
-  <si>
     <t>archivo_drive [FK] NOT NULL</t>
-  </si>
-  <si>
-    <t>id_liquidacion [FK] NOT NULL</t>
   </si>
 </sst>
 </file>
@@ -108,7 +99,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -162,17 +153,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -190,7 +170,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA5A6FF-93AF-D941-A4B0-25C7E9843D24}">
-  <dimension ref="B4:H9"/>
+  <dimension ref="B2:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -528,7 +508,17 @@
     <col min="14" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,11 +528,11 @@
       <c r="F4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
@@ -558,14 +548,11 @@
       <c r="F5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
@@ -575,33 +562,43 @@
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G6" s="6"/>
-      <c r="H6" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
terminamos de insertar datos
</commit_message>
<xml_diff>
--- a/modelo_lógico_datos_desafio_caso_1.xlsx
+++ b/modelo_lógico_datos_desafio_caso_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ariel/Desktop/desafiolatam/bases_de_datos_introducción/normalizacion_de_datos/modelos_desafio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38B1238-0E48-B640-851C-022D8C2CC591}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958403DD-1A75-A744-A34E-49D5DD54FCCA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="860" windowWidth="25040" windowHeight="14500" xr2:uid="{8EF448B2-BB9E-9141-B6BF-BD7A6BA49018}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>id SERIAL [PK]</t>
   </si>
   <si>
-    <t>rut INT [PK]</t>
-  </si>
-  <si>
     <t>nombre_departamento VARCHAR(100)</t>
   </si>
   <si>
@@ -57,13 +54,16 @@
     <t>direccion VARCHAR(200)</t>
   </si>
   <si>
-    <t>id_departamento [FK] NOT NULL</t>
-  </si>
-  <si>
     <t>rut_trabajador [FK] NOT NULL</t>
   </si>
   <si>
     <t>archivo_drive [FK] NOT NULL</t>
+  </si>
+  <si>
+    <t>rut VARCHAR(10) [PK]</t>
+  </si>
+  <si>
+    <t>id_departamento INT [FK] NOT NULL</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <dimension ref="B2:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -496,7 +496,7 @@
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="33.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="26.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" style="2"/>
@@ -540,7 +540,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>3</v>
@@ -554,15 +554,15 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -570,10 +570,10 @@
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -581,7 +581,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -589,7 +589,7 @@
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>

</xml_diff>